<commit_message>
New model results added
</commit_message>
<xml_diff>
--- a/results/4. NN_Regression/Data Set_NN.xlsx
+++ b/results/4. NN_Regression/Data Set_NN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GeonuKim\Desktop\ML project\Regression_Analysis_of_PECVD_SiNx\results\4. NN_Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B4978F-E1D4-43C2-AAE0-5713720D77CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E70C016D-D703-4BFD-A152-130B9CE5CC92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
   <si>
     <t>RF Freq (MHz)</t>
   </si>
@@ -68,44 +68,59 @@
     <t>Rand for Shuffle</t>
   </si>
   <si>
-    <t>Test1 (epoch=500)</t>
+    <t>Tensile Stress by NN_selected (Mpa)</t>
   </si>
   <si>
-    <t>Test2 (epoch=1000)</t>
+    <t>Test_(Epoch=1000, relu1-linear output)</t>
   </si>
   <si>
-    <t>Test3 (epoch=1500)</t>
+    <t>Test_(Epoch=1000, relu2-linear output)</t>
   </si>
   <si>
-    <t>Test4 (epoch=1500)</t>
+    <t>Test1 (epoch=500, linear1+linear output)</t>
   </si>
   <si>
-    <t>Test5 (epoch=2000)</t>
+    <t>Test2 (epoch=1000 ,linear1+linear output)</t>
   </si>
   <si>
-    <t>Test6 (epoch=1500)</t>
+    <t>Test3 (epoch=1500 ,linear1+linear output)</t>
   </si>
   <si>
-    <t>Test_a (epoch = 25)</t>
+    <t>Test4 (epoch=1500 ,linear1+linear output)</t>
   </si>
   <si>
-    <t>Test_b (epoch = 150)</t>
+    <t>Test5 (epoch=2000 ,linear1+linear output)</t>
   </si>
   <si>
-    <t>Test_c (epoch = 500)</t>
+    <t>Test6 (epoch=1500 ,linear1+linear output)</t>
   </si>
   <si>
-    <t>Test_d (epoch = 1000)</t>
+    <t>Test_a (epoch = 25 ,linear1+linear output)</t>
   </si>
   <si>
-    <t>Tensile Stress by NN_selected (Mpa)</t>
+    <t>Test_b (epoch = 150 ,linear1+linear output)</t>
+  </si>
+  <si>
+    <t>Test_c (epoch = 500 ,linear1+linear output)</t>
+  </si>
+  <si>
+    <t>Test_d (epoch = 1000 ,linear1+linear output)</t>
+  </si>
+  <si>
+    <t>Test_(Epoch=1000, tanh2-linear output)</t>
+  </si>
+  <si>
+    <t>Test_(Epoch=500, sigmoid2-linear output)</t>
+  </si>
+  <si>
+    <t>Test_(Epoch=1000, sigmoid2-linear output)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,6 +137,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -180,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -195,6 +217,7 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -753,7 +776,7 @@
                 <c:order val="3"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Shuffled_Rand_removed!$K$1</c15:sqref>
@@ -763,7 +786,7 @@
                     <c:strCache>
                       <c:ptCount val="1"/>
                       <c:pt idx="0">
-                        <c:v>Test1 (epoch=500)</c:v>
+                        <c:v>Test1 (epoch=500, linear1+linear output)</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -794,7 +817,7 @@
                 </c:marker>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Shuffled_Rand_removed!$K$2:$K$44</c15:sqref>
@@ -937,7 +960,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-7A9C-47C1-AEB9-4352A7A66580}"/>
                   </c:ext>
@@ -950,7 +973,7 @@
                 <c:order val="4"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Shuffled_Rand_removed!$L$1</c15:sqref>
@@ -960,7 +983,7 @@
                     <c:strCache>
                       <c:ptCount val="1"/>
                       <c:pt idx="0">
-                        <c:v>Test2 (epoch=1000)</c:v>
+                        <c:v>Test2 (epoch=1000 ,linear1+linear output)</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -991,7 +1014,7 @@
                 </c:marker>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Shuffled_Rand_removed!$L$2:$L$44</c15:sqref>
@@ -1134,7 +1157,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-7A9C-47C1-AEB9-4352A7A66580}"/>
                   </c:ext>
@@ -1147,7 +1170,7 @@
                 <c:order val="5"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Shuffled_Rand_removed!$M$1</c15:sqref>
@@ -1157,7 +1180,7 @@
                     <c:strCache>
                       <c:ptCount val="1"/>
                       <c:pt idx="0">
-                        <c:v>Test3 (epoch=1500)</c:v>
+                        <c:v>Test3 (epoch=1500 ,linear1+linear output)</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -1188,7 +1211,7 @@
                 </c:marker>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Shuffled_Rand_removed!$M$2:$M$44</c15:sqref>
@@ -1331,7 +1354,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000004-7A9C-47C1-AEB9-4352A7A66580}"/>
                   </c:ext>
@@ -1344,7 +1367,7 @@
                 <c:order val="6"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Shuffled_Rand_removed!$N$1</c15:sqref>
@@ -1354,7 +1377,7 @@
                     <c:strCache>
                       <c:ptCount val="1"/>
                       <c:pt idx="0">
-                        <c:v>Test4 (epoch=1500)</c:v>
+                        <c:v>Test4 (epoch=1500 ,linear1+linear output)</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -1391,7 +1414,7 @@
                 </c:marker>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Shuffled_Rand_removed!$N$2:$N$44</c15:sqref>
@@ -1534,7 +1557,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-7A9C-47C1-AEB9-4352A7A66580}"/>
                   </c:ext>
@@ -1547,7 +1570,7 @@
                 <c:order val="7"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Shuffled_Rand_removed!$O$1</c15:sqref>
@@ -1557,7 +1580,7 @@
                     <c:strCache>
                       <c:ptCount val="1"/>
                       <c:pt idx="0">
-                        <c:v>Test5 (epoch=2000)</c:v>
+                        <c:v>Test5 (epoch=2000 ,linear1+linear output)</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -1594,7 +1617,7 @@
                 </c:marker>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Shuffled_Rand_removed!$O$2:$O$44</c15:sqref>
@@ -1737,7 +1760,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000006-7A9C-47C1-AEB9-4352A7A66580}"/>
                   </c:ext>
@@ -1750,7 +1773,7 @@
                 <c:order val="8"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Shuffled_Rand_removed!$P$1</c15:sqref>
@@ -1760,7 +1783,7 @@
                     <c:strCache>
                       <c:ptCount val="1"/>
                       <c:pt idx="0">
-                        <c:v>Test6 (epoch=1500)</c:v>
+                        <c:v>Test6 (epoch=1500 ,linear1+linear output)</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -1797,7 +1820,7 @@
                 </c:marker>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Shuffled_Rand_removed!$P$2:$P$44</c15:sqref>
@@ -1940,7 +1963,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000007-7A9C-47C1-AEB9-4352A7A66580}"/>
                   </c:ext>
@@ -1953,7 +1976,7 @@
                 <c:order val="9"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Shuffled_Rand_removed!$Q$1</c15:sqref>
@@ -1997,7 +2020,7 @@
                 </c:marker>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Shuffled_Rand_removed!$Q$2:$Q$44</c15:sqref>
@@ -2011,7 +2034,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000008-7A9C-47C1-AEB9-4352A7A66580}"/>
                   </c:ext>
@@ -2024,7 +2047,7 @@
                 <c:order val="10"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Shuffled_Rand_removed!$R$1</c15:sqref>
@@ -2034,7 +2057,7 @@
                     <c:strCache>
                       <c:ptCount val="1"/>
                       <c:pt idx="0">
-                        <c:v>Test_a (epoch = 25)</c:v>
+                        <c:v>Test_a (epoch = 25 ,linear1+linear output)</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -2071,7 +2094,7 @@
                 </c:marker>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Shuffled_Rand_removed!$R$2:$R$44</c15:sqref>
@@ -2214,7 +2237,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000009-7A9C-47C1-AEB9-4352A7A66580}"/>
                   </c:ext>
@@ -2227,7 +2250,7 @@
                 <c:order val="11"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Shuffled_Rand_removed!$S$1</c15:sqref>
@@ -2237,7 +2260,7 @@
                     <c:strCache>
                       <c:ptCount val="1"/>
                       <c:pt idx="0">
-                        <c:v>Test_b (epoch = 150)</c:v>
+                        <c:v>Test_b (epoch = 150 ,linear1+linear output)</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -2274,7 +2297,7 @@
                 </c:marker>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Shuffled_Rand_removed!$S$2:$S$44</c15:sqref>
@@ -2417,7 +2440,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000A-7A9C-47C1-AEB9-4352A7A66580}"/>
                   </c:ext>
@@ -2430,7 +2453,7 @@
                 <c:order val="12"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Shuffled_Rand_removed!$T$1</c15:sqref>
@@ -2440,7 +2463,7 @@
                     <c:strCache>
                       <c:ptCount val="1"/>
                       <c:pt idx="0">
-                        <c:v>Test_c (epoch = 500)</c:v>
+                        <c:v>Test_c (epoch = 500 ,linear1+linear output)</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -2480,7 +2503,7 @@
                 </c:marker>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Shuffled_Rand_removed!$T$2:$T$44</c15:sqref>
@@ -2623,7 +2646,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000B-7A9C-47C1-AEB9-4352A7A66580}"/>
                   </c:ext>
@@ -2636,7 +2659,7 @@
                 <c:order val="13"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Shuffled_Rand_removed!$U$1</c15:sqref>
@@ -2646,7 +2669,7 @@
                     <c:strCache>
                       <c:ptCount val="1"/>
                       <c:pt idx="0">
-                        <c:v>Test_d (epoch = 1000)</c:v>
+                        <c:v>Test_d (epoch = 1000 ,linear1+linear output)</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -2686,7 +2709,7 @@
                 </c:marker>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Shuffled_Rand_removed!$U$2:$U$44</c15:sqref>
@@ -2829,7 +2852,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000C-7A9C-47C1-AEB9-4352A7A66580}"/>
                   </c:ext>
@@ -4566,7 +4589,7 @@
       <xdr:col>22</xdr:col>
       <xdr:colOff>580038</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>48026</xdr:rowOff>
+      <xdr:rowOff>59231</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
@@ -4587,10 +4610,10 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="14051109" y="5382026"/>
-          <a:ext cx="4069603" cy="3025587"/>
-          <a:chOff x="15248538" y="4728883"/>
-          <a:chExt cx="4069603" cy="3025587"/>
+          <a:off x="13892626" y="5393231"/>
+          <a:ext cx="4019177" cy="3014382"/>
+          <a:chOff x="15248538" y="4740088"/>
+          <a:chExt cx="4069603" cy="3014382"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:pic>
@@ -4635,8 +4658,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="15278419" y="4728883"/>
-            <a:ext cx="1460272" cy="264560"/>
+            <a:off x="16784320" y="6054100"/>
+            <a:ext cx="2249334" cy="264560"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -4669,7 +4692,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" sz="1100" baseline="0"/>
-              <a:t>_d (epoch = 1000)</a:t>
+              <a:t>_d (epoch = 1000, linear+linear)</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" sz="1100"/>
           </a:p>
@@ -4985,10 +5008,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3186E75-438A-4A95-88D4-48D169AD77DA}">
-  <dimension ref="A1:U89"/>
+  <dimension ref="A1:AA89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AE29" sqref="AE29"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AD3" sqref="AD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4998,9 +5021,10 @@
     <col min="12" max="12" width="9.140625" style="13"/>
     <col min="15" max="15" width="9.140625" style="5"/>
     <col min="16" max="16" width="9.140625" style="13"/>
+    <col min="25" max="25" width="9.140625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -5026,40 +5050,55 @@
         <v>7</v>
       </c>
       <c r="I1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="12" t="s">
+      <c r="T1" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="X1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="R1" t="s">
-        <v>15</v>
-      </c>
-      <c r="S1" t="s">
-        <v>16</v>
-      </c>
-      <c r="T1" t="s">
-        <v>17</v>
-      </c>
-      <c r="U1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Y1" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>13.56</v>
       </c>
@@ -5117,8 +5156,23 @@
       <c r="U2">
         <v>69.953469999999996</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W2">
+        <v>67.130859999999998</v>
+      </c>
+      <c r="X2">
+        <v>28.163869999999999</v>
+      </c>
+      <c r="Y2" s="14">
+        <v>50.758580000000002</v>
+      </c>
+      <c r="Z2">
+        <v>93.102806000000001</v>
+      </c>
+      <c r="AA2">
+        <v>62.245795999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>13.56</v>
       </c>
@@ -5176,8 +5230,23 @@
       <c r="U3">
         <v>56.783123000000003</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W3">
+        <v>56.824027999999998</v>
+      </c>
+      <c r="X3">
+        <v>45.574406000000003</v>
+      </c>
+      <c r="Y3" s="14">
+        <v>51.817473999999997</v>
+      </c>
+      <c r="Z3">
+        <v>78.367869999999996</v>
+      </c>
+      <c r="AA3">
+        <v>55.439563999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>13.56</v>
       </c>
@@ -5235,8 +5304,23 @@
       <c r="U4">
         <v>-7.098141</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W4">
+        <v>5.7159757999999998</v>
+      </c>
+      <c r="X4">
+        <v>7.4130963999999997</v>
+      </c>
+      <c r="Y4" s="14">
+        <v>-1.9750726999999999</v>
+      </c>
+      <c r="Z4">
+        <v>59.507730000000002</v>
+      </c>
+      <c r="AA4">
+        <v>2.5674996000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>13.56</v>
       </c>
@@ -5294,8 +5378,23 @@
       <c r="U5">
         <v>25.807048999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W5">
+        <v>29.001345000000001</v>
+      </c>
+      <c r="X5">
+        <v>38.954174000000002</v>
+      </c>
+      <c r="Y5" s="14">
+        <v>29.533655</v>
+      </c>
+      <c r="Z5">
+        <v>36.276203000000002</v>
+      </c>
+      <c r="AA5">
+        <v>26.609613</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>13.56</v>
       </c>
@@ -5353,8 +5452,23 @@
       <c r="U6">
         <v>35.140895999999998</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W6">
+        <v>35.580353000000002</v>
+      </c>
+      <c r="X6">
+        <v>24.292953000000001</v>
+      </c>
+      <c r="Y6" s="14">
+        <v>29.56776</v>
+      </c>
+      <c r="Z6">
+        <v>67.373999999999995</v>
+      </c>
+      <c r="AA6">
+        <v>36.262059999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>13.56</v>
       </c>
@@ -5412,8 +5526,23 @@
       <c r="U7">
         <v>25.258483999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W7">
+        <v>27.310321999999999</v>
+      </c>
+      <c r="X7">
+        <v>23.034673999999999</v>
+      </c>
+      <c r="Y7" s="14">
+        <v>20.050097999999998</v>
+      </c>
+      <c r="Z7">
+        <v>42.438133000000001</v>
+      </c>
+      <c r="AA7">
+        <v>39.7286</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>13.56</v>
       </c>
@@ -5471,8 +5600,23 @@
       <c r="U8">
         <v>83.984886000000003</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W8">
+        <v>88.104650000000007</v>
+      </c>
+      <c r="X8">
+        <v>110.45177</v>
+      </c>
+      <c r="Y8" s="14">
+        <v>107.40067000000001</v>
+      </c>
+      <c r="Z8">
+        <v>81.94211</v>
+      </c>
+      <c r="AA8">
+        <v>80.102339999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>13.56</v>
       </c>
@@ -5530,8 +5674,23 @@
       <c r="U9">
         <v>29.135252000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W9">
+        <v>31.829658999999999</v>
+      </c>
+      <c r="X9">
+        <v>31.526688</v>
+      </c>
+      <c r="Y9" s="14">
+        <v>27.285309999999999</v>
+      </c>
+      <c r="Z9">
+        <v>35.104669999999999</v>
+      </c>
+      <c r="AA9">
+        <v>37.163722999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>13.56</v>
       </c>
@@ -5589,8 +5748,23 @@
       <c r="U10">
         <v>104.22996000000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W10">
+        <v>105.09617</v>
+      </c>
+      <c r="X10">
+        <v>116.19670000000001</v>
+      </c>
+      <c r="Y10" s="14">
+        <v>107.21413</v>
+      </c>
+      <c r="Z10">
+        <v>90.630250000000004</v>
+      </c>
+      <c r="AA10">
+        <v>101.90671</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>13.56</v>
       </c>
@@ -5648,8 +5822,23 @@
       <c r="U11">
         <v>26.429966</v>
       </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W11">
+        <v>29.571905000000001</v>
+      </c>
+      <c r="X11">
+        <v>30.25151</v>
+      </c>
+      <c r="Y11" s="14">
+        <v>37.489165999999997</v>
+      </c>
+      <c r="Z11">
+        <v>58.722023</v>
+      </c>
+      <c r="AA11">
+        <v>25.117833999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>13.56</v>
       </c>
@@ -5707,8 +5896,23 @@
       <c r="U12">
         <v>18.269546999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W12">
+        <v>21.301445000000001</v>
+      </c>
+      <c r="X12">
+        <v>25.582453000000001</v>
+      </c>
+      <c r="Y12" s="14">
+        <v>24.211760000000002</v>
+      </c>
+      <c r="Z12">
+        <v>45.344757000000001</v>
+      </c>
+      <c r="AA12">
+        <v>18.471405000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>13.56</v>
       </c>
@@ -5766,8 +5970,23 @@
       <c r="U13">
         <v>85.878630000000001</v>
       </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W13">
+        <v>87.944829999999996</v>
+      </c>
+      <c r="X13">
+        <v>103.85251</v>
+      </c>
+      <c r="Y13" s="14">
+        <v>95.626310000000004</v>
+      </c>
+      <c r="Z13">
+        <v>86.08005</v>
+      </c>
+      <c r="AA13">
+        <v>86.436459999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>13.56</v>
       </c>
@@ -5825,8 +6044,23 @@
       <c r="U14">
         <v>100.2433</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W14">
+        <v>102.55354</v>
+      </c>
+      <c r="X14">
+        <v>123.86903</v>
+      </c>
+      <c r="Y14" s="14">
+        <v>112.87454</v>
+      </c>
+      <c r="Z14">
+        <v>92.224010000000007</v>
+      </c>
+      <c r="AA14">
+        <v>100.33383000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>13.56</v>
       </c>
@@ -5884,8 +6118,23 @@
       <c r="U15">
         <v>85.322013999999996</v>
       </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W15">
+        <v>85.84778</v>
+      </c>
+      <c r="X15">
+        <v>85.342100000000002</v>
+      </c>
+      <c r="Y15" s="14">
+        <v>86.568404999999998</v>
+      </c>
+      <c r="Z15">
+        <v>90.404750000000007</v>
+      </c>
+      <c r="AA15">
+        <v>82.974884000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>13.56</v>
       </c>
@@ -5943,8 +6192,23 @@
       <c r="U16">
         <v>46.576282999999997</v>
       </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W16">
+        <v>78.236176</v>
+      </c>
+      <c r="X16">
+        <v>36.526893999999999</v>
+      </c>
+      <c r="Y16" s="14">
+        <v>60.395150000000001</v>
+      </c>
+      <c r="Z16">
+        <v>45.011310000000002</v>
+      </c>
+      <c r="AA16">
+        <v>26.876588999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>13.56</v>
       </c>
@@ -6002,8 +6266,23 @@
       <c r="U17">
         <v>71.402370000000005</v>
       </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W17">
+        <v>73.222626000000005</v>
+      </c>
+      <c r="X17">
+        <v>83.680459999999997</v>
+      </c>
+      <c r="Y17" s="14">
+        <v>78.111199999999997</v>
+      </c>
+      <c r="Z17">
+        <v>79.994119999999995</v>
+      </c>
+      <c r="AA17">
+        <v>72.430274999999995</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>13.56</v>
       </c>
@@ -6061,8 +6340,23 @@
       <c r="U18">
         <v>99.606449999999995</v>
       </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W18">
+        <v>100.374886</v>
+      </c>
+      <c r="X18">
+        <v>105.24684000000001</v>
+      </c>
+      <c r="Y18" s="14">
+        <v>103.80364</v>
+      </c>
+      <c r="Z18">
+        <v>96.582436000000001</v>
+      </c>
+      <c r="AA18">
+        <v>96.799809999999994</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>13.56</v>
       </c>
@@ -6120,8 +6414,23 @@
       <c r="U19">
         <v>65.716250000000002</v>
       </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W19">
+        <v>63.290675999999998</v>
+      </c>
+      <c r="X19">
+        <v>27.692716999999998</v>
+      </c>
+      <c r="Y19" s="14">
+        <v>48.18233</v>
+      </c>
+      <c r="Z19">
+        <v>89.865849999999995</v>
+      </c>
+      <c r="AA19">
+        <v>59.059249999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>13.56</v>
       </c>
@@ -6179,8 +6488,23 @@
       <c r="U20">
         <v>33.106340000000003</v>
       </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W20">
+        <v>36.458959999999998</v>
+      </c>
+      <c r="X20">
+        <v>40.225304000000001</v>
+      </c>
+      <c r="Y20" s="14">
+        <v>34.694415999999997</v>
+      </c>
+      <c r="Z20">
+        <v>27.866015999999998</v>
+      </c>
+      <c r="AA20">
+        <v>34.545096999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>13.56</v>
       </c>
@@ -6238,8 +6562,23 @@
       <c r="U21">
         <v>46.318035000000002</v>
       </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W21">
+        <v>46.200375000000001</v>
+      </c>
+      <c r="X21">
+        <v>35.474789999999999</v>
+      </c>
+      <c r="Y21" s="14">
+        <v>36.805059999999997</v>
+      </c>
+      <c r="Z21">
+        <v>66.634799999999998</v>
+      </c>
+      <c r="AA21">
+        <v>46.071423000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>13.56</v>
       </c>
@@ -6297,8 +6636,23 @@
       <c r="U22">
         <v>28.180340000000001</v>
       </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W22">
+        <v>29.266283000000001</v>
+      </c>
+      <c r="X22">
+        <v>23.452456000000002</v>
+      </c>
+      <c r="Y22" s="14">
+        <v>25.294197</v>
+      </c>
+      <c r="Z22">
+        <v>62.495026000000003</v>
+      </c>
+      <c r="AA22">
+        <v>31.124233</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>13.56</v>
       </c>
@@ -6356,8 +6710,23 @@
       <c r="U23">
         <v>62.780895000000001</v>
       </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W23">
+        <v>60.630367</v>
+      </c>
+      <c r="X23">
+        <v>27.366333000000001</v>
+      </c>
+      <c r="Y23" s="14">
+        <v>46.397019999999998</v>
+      </c>
+      <c r="Z23">
+        <v>87.639759999999995</v>
+      </c>
+      <c r="AA23">
+        <v>56.854874000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>13.56</v>
       </c>
@@ -6415,8 +6784,23 @@
       <c r="U24">
         <v>60.595073999999997</v>
       </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W24">
+        <v>60.719974999999998</v>
+      </c>
+      <c r="X24">
+        <v>55.393410000000003</v>
+      </c>
+      <c r="Y24" s="14">
+        <v>54.288969999999999</v>
+      </c>
+      <c r="Z24">
+        <v>72.382773999999998</v>
+      </c>
+      <c r="AA24">
+        <v>59.739821999999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>13.56</v>
       </c>
@@ -6474,8 +6858,23 @@
       <c r="U25">
         <v>89.348849999999999</v>
       </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W25">
+        <v>89.962233999999995</v>
+      </c>
+      <c r="X25">
+        <v>95.460520000000002</v>
+      </c>
+      <c r="Y25" s="14">
+        <v>89.279526000000004</v>
+      </c>
+      <c r="Z25">
+        <v>84.295974999999999</v>
+      </c>
+      <c r="AA25">
+        <v>87.512985</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>13.56</v>
       </c>
@@ -6533,8 +6932,23 @@
       <c r="U26">
         <v>10.913197</v>
       </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W26">
+        <v>13.786612</v>
+      </c>
+      <c r="X26">
+        <v>7.4770545999999998</v>
+      </c>
+      <c r="Y26" s="14">
+        <v>19.016966</v>
+      </c>
+      <c r="Z26">
+        <v>54.570144999999997</v>
+      </c>
+      <c r="AA26">
+        <v>10.606617999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>13.56</v>
       </c>
@@ -6592,8 +7006,23 @@
       <c r="U27">
         <v>74.771100000000004</v>
       </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W27">
+        <v>75.136840000000007</v>
+      </c>
+      <c r="X27">
+        <v>75.147069999999999</v>
+      </c>
+      <c r="Y27" s="14">
+        <v>71.586044000000001</v>
+      </c>
+      <c r="Z27">
+        <v>78.201096000000007</v>
+      </c>
+      <c r="AA27">
+        <v>73.408280000000005</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>13.56</v>
       </c>
@@ -6651,8 +7080,23 @@
       <c r="U28">
         <v>71.068809999999999</v>
       </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W28">
+        <v>71.352419999999995</v>
+      </c>
+      <c r="X28">
+        <v>65.480890000000002</v>
+      </c>
+      <c r="Y28" s="14">
+        <v>69.256609999999995</v>
+      </c>
+      <c r="Z28">
+        <v>84.34084</v>
+      </c>
+      <c r="AA28">
+        <v>69.191779999999994</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>13.56</v>
       </c>
@@ -6710,8 +7154,23 @@
       <c r="U29">
         <v>11.141788999999999</v>
       </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W29">
+        <v>14.180918</v>
+      </c>
+      <c r="X29">
+        <v>7.7026896000000002</v>
+      </c>
+      <c r="Y29" s="14">
+        <v>19.272165000000001</v>
+      </c>
+      <c r="Z29">
+        <v>54.483580000000003</v>
+      </c>
+      <c r="AA29">
+        <v>10.72433</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>13.56</v>
       </c>
@@ -6769,8 +7228,23 @@
       <c r="U30">
         <v>118.709946</v>
       </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W30">
+        <v>119.822174</v>
+      </c>
+      <c r="X30">
+        <v>136.37393</v>
+      </c>
+      <c r="Y30" s="14">
+        <v>124.51461999999999</v>
+      </c>
+      <c r="Z30">
+        <v>96.898229999999998</v>
+      </c>
+      <c r="AA30">
+        <v>115.85384000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>13.56</v>
       </c>
@@ -6828,8 +7302,23 @@
       <c r="U31">
         <v>33.232353000000003</v>
       </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W31">
+        <v>36.586620000000003</v>
+      </c>
+      <c r="X31">
+        <v>40.23207</v>
+      </c>
+      <c r="Y31" s="14">
+        <v>34.774765000000002</v>
+      </c>
+      <c r="Z31">
+        <v>27.729074000000001</v>
+      </c>
+      <c r="AA31">
+        <v>34.695796999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>13.56</v>
       </c>
@@ -6887,8 +7376,23 @@
       <c r="U32">
         <v>114.37157000000001</v>
       </c>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W32">
+        <v>115.39085</v>
+      </c>
+      <c r="X32">
+        <v>125.821365</v>
+      </c>
+      <c r="Y32" s="14">
+        <v>121.471</v>
+      </c>
+      <c r="Z32">
+        <v>103.06873</v>
+      </c>
+      <c r="AA32">
+        <v>111.04809</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>13.56</v>
       </c>
@@ -6946,8 +7450,23 @@
       <c r="U33">
         <v>69.737755000000007</v>
       </c>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W33">
+        <v>73.615470000000002</v>
+      </c>
+      <c r="X33">
+        <v>90.599000000000004</v>
+      </c>
+      <c r="Y33" s="14">
+        <v>90.252529999999993</v>
+      </c>
+      <c r="Z33">
+        <v>76.024479999999997</v>
+      </c>
+      <c r="AA33">
+        <v>66.332610000000003</v>
+      </c>
+    </row>
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>13.56</v>
       </c>
@@ -7005,8 +7524,23 @@
       <c r="U34">
         <v>39.645114999999997</v>
       </c>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W34">
+        <v>44.081530000000001</v>
+      </c>
+      <c r="X34">
+        <v>54.548411999999999</v>
+      </c>
+      <c r="Y34" s="14">
+        <v>46.882435000000001</v>
+      </c>
+      <c r="Z34">
+        <v>16.554237000000001</v>
+      </c>
+      <c r="AA34">
+        <v>30.253632</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>13.56</v>
       </c>
@@ -7064,8 +7598,23 @@
       <c r="U35">
         <v>40.900475</v>
       </c>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W35">
+        <v>44.288272999999997</v>
+      </c>
+      <c r="X35">
+        <v>50.415529999999997</v>
+      </c>
+      <c r="Y35" s="14">
+        <v>55.198321999999997</v>
+      </c>
+      <c r="Z35">
+        <v>64.385249999999999</v>
+      </c>
+      <c r="AA35">
+        <v>38.731670000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>13.56</v>
       </c>
@@ -7123,8 +7672,23 @@
       <c r="U36">
         <v>42.564390000000003</v>
       </c>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W36">
+        <v>43.8947</v>
+      </c>
+      <c r="X36">
+        <v>43.495989999999999</v>
+      </c>
+      <c r="Y36" s="14">
+        <v>42.930250000000001</v>
+      </c>
+      <c r="Z36">
+        <v>68.203299999999999</v>
+      </c>
+      <c r="AA36">
+        <v>44.734817999999997</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>13.56</v>
       </c>
@@ -7182,8 +7746,23 @@
       <c r="U37">
         <v>12.0617695</v>
       </c>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W37">
+        <v>14.959605</v>
+      </c>
+      <c r="X37">
+        <v>10.230059000000001</v>
+      </c>
+      <c r="Y37" s="14">
+        <v>19.864125999999999</v>
+      </c>
+      <c r="Z37">
+        <v>53.219856</v>
+      </c>
+      <c r="AA37">
+        <v>11.818873999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>13.56</v>
       </c>
@@ -7241,8 +7820,23 @@
       <c r="U38">
         <v>42.319522999999997</v>
       </c>
-    </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W38">
+        <v>42.114699999999999</v>
+      </c>
+      <c r="X38">
+        <v>25.420006000000001</v>
+      </c>
+      <c r="Y38" s="14">
+        <v>34.099457000000001</v>
+      </c>
+      <c r="Z38">
+        <v>72.431434999999993</v>
+      </c>
+      <c r="AA38">
+        <v>41.630465999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>13.56</v>
       </c>
@@ -7300,8 +7894,23 @@
       <c r="U39">
         <v>-24.567781</v>
       </c>
-    </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W39">
+        <v>5.7159757999999998</v>
+      </c>
+      <c r="X39">
+        <v>7.4130963999999997</v>
+      </c>
+      <c r="Y39" s="14">
+        <v>-22.288371999999999</v>
+      </c>
+      <c r="Z39">
+        <v>64.412170000000003</v>
+      </c>
+      <c r="AA39">
+        <v>-5.1312813999999998</v>
+      </c>
+    </row>
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>13.56</v>
       </c>
@@ -7359,8 +7968,23 @@
       <c r="U40">
         <v>55.265790000000003</v>
       </c>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W40">
+        <v>58.897640000000003</v>
+      </c>
+      <c r="X40">
+        <v>70.432959999999994</v>
+      </c>
+      <c r="Y40" s="14">
+        <v>72.709370000000007</v>
+      </c>
+      <c r="Z40">
+        <v>70.125559999999993</v>
+      </c>
+      <c r="AA40">
+        <v>52.419020000000003</v>
+      </c>
+    </row>
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>13.56</v>
       </c>
@@ -7418,8 +8042,23 @@
       <c r="U41">
         <v>56.023769999999999</v>
       </c>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W41">
+        <v>54.506416000000002</v>
+      </c>
+      <c r="X41">
+        <v>26.614985999999998</v>
+      </c>
+      <c r="Y41" s="14">
+        <v>42.285572000000002</v>
+      </c>
+      <c r="Z41">
+        <v>82.567530000000005</v>
+      </c>
+      <c r="AA41">
+        <v>51.791289999999996</v>
+      </c>
+    </row>
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>13.56</v>
       </c>
@@ -7477,8 +8116,23 @@
       <c r="U42">
         <v>28.689596000000002</v>
       </c>
-    </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W42">
+        <v>45.902250000000002</v>
+      </c>
+      <c r="X42">
+        <v>21.976956999999999</v>
+      </c>
+      <c r="Y42" s="14">
+        <v>39.684227</v>
+      </c>
+      <c r="Z42">
+        <v>49.744729999999997</v>
+      </c>
+      <c r="AA42">
+        <v>18.676207999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>13.56</v>
       </c>
@@ -7536,8 +8190,23 @@
       <c r="U43">
         <v>57.235218000000003</v>
       </c>
-    </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W43">
+        <v>58.814785000000001</v>
+      </c>
+      <c r="X43">
+        <v>63.939155999999997</v>
+      </c>
+      <c r="Y43" s="14">
+        <v>60.866936000000003</v>
+      </c>
+      <c r="Z43">
+        <v>74.145039999999995</v>
+      </c>
+      <c r="AA43">
+        <v>58.773086999999997</v>
+      </c>
+    </row>
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>13.56</v>
       </c>
@@ -7595,17 +8264,32 @@
       <c r="U44">
         <v>14.260106</v>
       </c>
-    </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W44">
+        <v>16.656178000000001</v>
+      </c>
+      <c r="X44">
+        <v>21.971147999999999</v>
+      </c>
+      <c r="Y44" s="14">
+        <v>16.842517999999998</v>
+      </c>
+      <c r="Z44">
+        <v>52.955880000000001</v>
+      </c>
+      <c r="AA44">
+        <v>20.969750000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="O45"/>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="O46"/>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="O47"/>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="O48"/>
     </row>
     <row r="49" spans="15:15" x14ac:dyDescent="0.25">
@@ -7773,7 +8457,7 @@
       </c>
       <c r="I2">
         <f t="shared" ref="I2:I44" ca="1" si="0">RAND()</f>
-        <v>0.33380799838948216</v>
+        <v>0.15252032563631535</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -7803,7 +8487,7 @@
       </c>
       <c r="I3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.15337510056930193</v>
+        <v>0.32726552541083331</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -7833,7 +8517,7 @@
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.46736920879814803</v>
+        <v>0.44560094581862331</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -7863,7 +8547,7 @@
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.62012249679712861</v>
+        <v>0.9008166669965697</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -7893,7 +8577,7 @@
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.79948507369738875</v>
+        <v>0.45657986040876009</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -7923,7 +8607,7 @@
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.92401321718257567</v>
+        <v>0.72151865428245665</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -7953,7 +8637,7 @@
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.97704890952332135</v>
+        <v>0.69808460586488574</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -7983,7 +8667,7 @@
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="0"/>
-        <v>0.39055860043098356</v>
+        <v>0.79250702145970164</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -8013,7 +8697,7 @@
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="0"/>
-        <v>0.7972431804069533</v>
+        <v>0.50876647695786559</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -8043,7 +8727,7 @@
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.90666897981271732</v>
+        <v>0.13713038038578074</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -8073,7 +8757,7 @@
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.40288911049271792</v>
+        <v>0.63303532280035779</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -8103,7 +8787,7 @@
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.86662905059653961</v>
+        <v>0.55203669462912897</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -8133,7 +8817,7 @@
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="0"/>
-        <v>0.83520682122096745</v>
+        <v>1.2895775360759365E-2</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -8163,7 +8847,7 @@
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="0"/>
-        <v>0.48348986733567001</v>
+        <v>0.12765860051165112</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -8193,7 +8877,7 @@
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.21610470167108187</v>
+        <v>0.95934291564808705</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -8223,7 +8907,7 @@
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="0"/>
-        <v>0.18470643644271756</v>
+        <v>7.2951753904390237E-2</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -8253,7 +8937,7 @@
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="0"/>
-        <v>0.68316240570049402</v>
+        <v>0.11278695933538763</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -8283,7 +8967,7 @@
       </c>
       <c r="I19">
         <f t="shared" ca="1" si="0"/>
-        <v>0.23135492150609926</v>
+        <v>0.19845404532203181</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -8313,7 +8997,7 @@
       </c>
       <c r="I20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.31756694317541412</v>
+        <v>0.48168721162276174</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -8343,7 +9027,7 @@
       </c>
       <c r="I21">
         <f t="shared" ca="1" si="0"/>
-        <v>0.2851553790485104</v>
+        <v>0.82256536711535677</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -8373,7 +9057,7 @@
       </c>
       <c r="I22">
         <f t="shared" ca="1" si="0"/>
-        <v>0.90817293265608123</v>
+        <v>0.68307828759905942</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -8403,7 +9087,7 @@
       </c>
       <c r="I23">
         <f t="shared" ca="1" si="0"/>
-        <v>0.67730261522782831</v>
+        <v>0.34934770550748262</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -8433,7 +9117,7 @@
       </c>
       <c r="I24">
         <f t="shared" ca="1" si="0"/>
-        <v>0.56312756125690411</v>
+        <v>3.8260067663560715E-2</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -8463,7 +9147,7 @@
       </c>
       <c r="I25">
         <f t="shared" ca="1" si="0"/>
-        <v>0.51855195570295998</v>
+        <v>0.17451740046405539</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -8493,7 +9177,7 @@
       </c>
       <c r="I26">
         <f t="shared" ca="1" si="0"/>
-        <v>0.13062495150437314</v>
+        <v>0.16338059206960553</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -8523,7 +9207,7 @@
       </c>
       <c r="I27">
         <f t="shared" ca="1" si="0"/>
-        <v>0.55374594151157996</v>
+        <v>0.27099048405155279</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -8553,7 +9237,7 @@
       </c>
       <c r="I28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.8898262581414853</v>
+        <v>0.73153415386367093</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -8583,7 +9267,7 @@
       </c>
       <c r="I29">
         <f t="shared" ca="1" si="0"/>
-        <v>0.91553247979539387</v>
+        <v>0.29700278302329086</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -8613,7 +9297,7 @@
       </c>
       <c r="I30">
         <f t="shared" ca="1" si="0"/>
-        <v>3.1944717420710034E-2</v>
+        <v>0.95248291542759789</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -8643,7 +9327,7 @@
       </c>
       <c r="I31">
         <f t="shared" ca="1" si="0"/>
-        <v>0.64308147392241766</v>
+        <v>0.25584475923431294</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -8673,7 +9357,7 @@
       </c>
       <c r="I32">
         <f t="shared" ca="1" si="0"/>
-        <v>0.33500370448811145</v>
+        <v>0.71970204579366981</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -8703,7 +9387,7 @@
       </c>
       <c r="I33">
         <f t="shared" ca="1" si="0"/>
-        <v>0.73406494976506664</v>
+        <v>0.91743958642646983</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -8733,7 +9417,7 @@
       </c>
       <c r="I34">
         <f t="shared" ca="1" si="0"/>
-        <v>0.32469959232036549</v>
+        <v>0.37801156553694837</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -8763,7 +9447,7 @@
       </c>
       <c r="I35">
         <f t="shared" ca="1" si="0"/>
-        <v>0.73073851462843598</v>
+        <v>2.1596962088439198E-2</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -8793,7 +9477,7 @@
       </c>
       <c r="I36">
         <f t="shared" ca="1" si="0"/>
-        <v>0.63116335490507702</v>
+        <v>0.97379404397644764</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -8823,7 +9507,7 @@
       </c>
       <c r="I37">
         <f t="shared" ca="1" si="0"/>
-        <v>0.8404986327423829</v>
+        <v>0.50691869620005059</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -8853,7 +9537,7 @@
       </c>
       <c r="I38">
         <f t="shared" ca="1" si="0"/>
-        <v>0.88621557517049954</v>
+        <v>0.2327361807211753</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -8883,7 +9567,7 @@
       </c>
       <c r="I39">
         <f t="shared" ca="1" si="0"/>
-        <v>0.56378181291165907</v>
+        <v>0.22888086335642233</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -8913,7 +9597,7 @@
       </c>
       <c r="I40">
         <f t="shared" ca="1" si="0"/>
-        <v>0.2243283190491614</v>
+        <v>0.26426330475224813</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -8943,7 +9627,7 @@
       </c>
       <c r="I41">
         <f t="shared" ca="1" si="0"/>
-        <v>0.27135890323843592</v>
+        <v>0.10504211519401152</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -8973,7 +9657,7 @@
       </c>
       <c r="I42">
         <f t="shared" ca="1" si="0"/>
-        <v>0.54564747914135792</v>
+        <v>0.46506509724437761</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -9003,7 +9687,7 @@
       </c>
       <c r="I43">
         <f t="shared" ca="1" si="0"/>
-        <v>0.45092800377550146</v>
+        <v>0.96698291924064073</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -9033,7 +9717,7 @@
       </c>
       <c r="I44">
         <f t="shared" ca="1" si="0"/>
-        <v>0.10432968861264669</v>
+        <v>0.26820217308197492</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
New Model and Results Added
</commit_message>
<xml_diff>
--- a/results/4. NN_Regression/Data Set_NN.xlsx
+++ b/results/4. NN_Regression/Data Set_NN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GeonuKim\Desktop\ML project\Regression_Analysis_of_PECVD_SiNx\results\4. NN_Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A660DCF8-7282-4A8B-BFD4-81CBCC50764B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C49AA6-3495-4D3B-A5D8-1F21B4740052}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="690" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Shuffled_Rand_removed" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
   <si>
     <t>RF Freq (MHz)</t>
   </si>
@@ -124,6 +124,9 @@
   <si>
     <t>Test_(Epoch=3000, tanh3-linear output)</t>
   </si>
+  <si>
+    <t>Test_by_NN_Model_Ver1.1</t>
+  </si>
 </sst>
 </file>
 
@@ -166,12 +169,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -219,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -237,6 +246,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -5027,10 +5037,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3186E75-438A-4A95-88D4-48D169AD77DA}">
-  <dimension ref="A1:AE89"/>
+  <dimension ref="A1:AG89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AG5" sqref="AG5"/>
+      <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5042,9 +5052,10 @@
     <col min="16" max="16" width="9.140625" style="16"/>
     <col min="25" max="25" width="9.140625" style="12"/>
     <col min="28" max="28" width="9.140625" customWidth="1"/>
+    <col min="33" max="33" width="9.140625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -5126,8 +5137,11 @@
       <c r="AE1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AG1" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>13.56</v>
       </c>
@@ -5209,8 +5223,11 @@
       <c r="AE2">
         <v>207.3518</v>
       </c>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AG2" s="17">
+        <v>68.751419999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>13.56</v>
       </c>
@@ -5292,8 +5309,11 @@
       <c r="AE3">
         <v>39.2361</v>
       </c>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AG3" s="17">
+        <v>55.454532999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>13.56</v>
       </c>
@@ -5375,8 +5395,11 @@
       <c r="AE4">
         <v>-6.9893226999999998</v>
       </c>
-    </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AG4" s="17">
+        <v>-5.3729706000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>13.56</v>
       </c>
@@ -5458,8 +5481,11 @@
       <c r="AE5">
         <v>33.665585</v>
       </c>
-    </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AG5" s="17">
+        <v>22.294035000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>13.56</v>
       </c>
@@ -5541,8 +5567,11 @@
       <c r="AE6">
         <v>5.6255474000000003</v>
       </c>
-    </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AG6" s="17">
+        <v>33.027996000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>13.56</v>
       </c>
@@ -5624,8 +5653,11 @@
       <c r="AE7">
         <v>33.435851999999997</v>
       </c>
-    </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AG7" s="17">
+        <v>34.922671999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>13.56</v>
       </c>
@@ -5707,8 +5739,11 @@
       <c r="AE8">
         <v>128.8236</v>
       </c>
-    </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AG8" s="17">
+        <v>126.76423</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>13.56</v>
       </c>
@@ -5790,8 +5825,11 @@
       <c r="AE9">
         <v>37.107635000000002</v>
       </c>
-    </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AG9" s="17">
+        <v>30.668865</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>13.56</v>
       </c>
@@ -5873,8 +5911,11 @@
       <c r="AE10">
         <v>91.48075</v>
       </c>
-    </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AG10" s="17">
+        <v>112.17992</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>13.56</v>
       </c>
@@ -5956,8 +5997,11 @@
       <c r="AE11">
         <v>31.856639999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AG11" s="17">
+        <v>27.497883000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>13.56</v>
       </c>
@@ -6039,8 +6083,11 @@
       <c r="AE12">
         <v>18.830825999999998</v>
       </c>
-    </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AG12" s="17">
+        <v>13.376815000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>13.56</v>
       </c>
@@ -6122,8 +6169,11 @@
       <c r="AE13">
         <v>89.294579999999996</v>
       </c>
-    </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AG13" s="17">
+        <v>100.48035</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>13.56</v>
       </c>
@@ -6205,8 +6255,11 @@
       <c r="AE14">
         <v>107.54058000000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AG14" s="17">
+        <v>122.66893</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>13.56</v>
       </c>
@@ -6288,8 +6341,11 @@
       <c r="AE15">
         <v>88.703419999999994</v>
       </c>
-    </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AG15" s="17">
+        <v>88.287270000000007</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>13.56</v>
       </c>
@@ -6371,8 +6427,11 @@
       <c r="AE16">
         <v>26.748857000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AG16" s="17">
+        <v>24.917252999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>13.56</v>
       </c>
@@ -6454,8 +6513,11 @@
       <c r="AE17">
         <v>69.9499</v>
       </c>
-    </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AG17" s="17">
+        <v>79.326099999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>13.56</v>
       </c>
@@ -6537,8 +6599,11 @@
       <c r="AE18">
         <v>112.35636</v>
       </c>
-    </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AG18" s="17">
+        <v>106.89429</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>13.56</v>
       </c>
@@ -6620,8 +6685,11 @@
       <c r="AE19">
         <v>154.14319</v>
       </c>
-    </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AG19" s="17">
+        <v>64.694360000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>13.56</v>
       </c>
@@ -6703,8 +6771,11 @@
       <c r="AE20">
         <v>40.443874000000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AG20" s="17">
+        <v>30.91028</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>13.56</v>
       </c>
@@ -6786,8 +6857,11 @@
       <c r="AE21">
         <v>7.2372569999999996</v>
       </c>
-    </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AG21" s="17">
+        <v>45.266629999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>13.56</v>
       </c>
@@ -6869,8 +6943,11 @@
       <c r="AE22">
         <v>5.8224735000000001</v>
       </c>
-    </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AG22" s="17">
+        <v>25.980103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>13.56</v>
       </c>
@@ -6952,8 +7029,11 @@
       <c r="AE23">
         <v>122.44323</v>
       </c>
-    </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AG23" s="17">
+        <v>61.799045999999997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>13.56</v>
       </c>
@@ -7035,8 +7115,11 @@
       <c r="AE24">
         <v>29.396135000000001</v>
       </c>
-    </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AG24" s="17">
+        <v>59.996014000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>13.56</v>
       </c>
@@ -7118,8 +7201,11 @@
       <c r="AE25">
         <v>71.184610000000006</v>
       </c>
-    </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AG25" s="17">
+        <v>92.902169999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>13.56</v>
       </c>
@@ -7201,8 +7287,11 @@
       <c r="AE26">
         <v>3.3650427000000001</v>
       </c>
-    </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AG26" s="17">
+        <v>4.6627280000000004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>13.56</v>
       </c>
@@ -7284,8 +7373,11 @@
       <c r="AE27">
         <v>50.450355999999999</v>
       </c>
-    </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AG27" s="17">
+        <v>75.546239999999997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>13.56</v>
       </c>
@@ -7367,8 +7459,11 @@
       <c r="AE28">
         <v>64.388599999999997</v>
       </c>
-    </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AG28" s="17">
+        <v>71.204864999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>13.56</v>
       </c>
@@ -7450,8 +7545,11 @@
       <c r="AE29">
         <v>3.5262753999999998</v>
       </c>
-    </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AG29" s="17">
+        <v>4.8061290000000003</v>
+      </c>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>13.56</v>
       </c>
@@ -7533,8 +7631,11 @@
       <c r="AE30">
         <v>110.48479</v>
       </c>
-    </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AG30" s="17">
+        <v>132.30789999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>13.56</v>
       </c>
@@ -7616,8 +7717,11 @@
       <c r="AE31">
         <v>40.481555999999998</v>
       </c>
-    </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AG31" s="17">
+        <v>31.062002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>13.56</v>
       </c>
@@ -7699,8 +7803,11 @@
       <c r="AE32">
         <v>136.14152999999999</v>
       </c>
-    </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AG32" s="17">
+        <v>127.54550999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>13.56</v>
       </c>
@@ -7782,8 +7889,11 @@
       <c r="AE33">
         <v>106.22513600000001</v>
       </c>
-    </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AG33" s="17">
+        <v>101.22172500000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>13.56</v>
       </c>
@@ -7865,8 +7975,11 @@
       <c r="AE34">
         <v>46.759341999999997</v>
       </c>
-    </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AG34" s="17">
+        <v>43.221989999999998</v>
+      </c>
+    </row>
+    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>13.56</v>
       </c>
@@ -7948,8 +8061,11 @@
       <c r="AE35">
         <v>57.672305999999999</v>
       </c>
-    </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AG35" s="17">
+        <v>50.949820000000003</v>
+      </c>
+    </row>
+    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>13.56</v>
       </c>
@@ -8031,8 +8147,11 @@
       <c r="AE36">
         <v>28.271229000000002</v>
       </c>
-    </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AG36" s="17">
+        <v>42.059852999999997</v>
+      </c>
+    </row>
+    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>13.56</v>
       </c>
@@ -8114,8 +8233,11 @@
       <c r="AE37">
         <v>5.2912306999999998</v>
       </c>
-    </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AG37" s="17">
+        <v>6.0401315999999996</v>
+      </c>
+    </row>
+    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>13.56</v>
       </c>
@@ -8197,8 +8319,11 @@
       <c r="AE38">
         <v>12.925604999999999</v>
       </c>
-    </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AG38" s="17">
+        <v>40.512529999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>13.56</v>
       </c>
@@ -8280,8 +8405,11 @@
       <c r="AE39">
         <v>-15.721045500000001</v>
       </c>
-    </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AG39" s="17">
+        <v>-14.991389</v>
+      </c>
+    </row>
+    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>13.56</v>
       </c>
@@ -8363,8 +8491,11 @@
       <c r="AE40">
         <v>82.339690000000004</v>
       </c>
-    </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AG40" s="17">
+        <v>75.581695999999994</v>
+      </c>
+    </row>
+    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>13.56</v>
       </c>
@@ -8446,8 +8577,11 @@
       <c r="AE41">
         <v>66.393814000000006</v>
       </c>
-    </row>
-    <row r="42" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AG41" s="17">
+        <v>54.924610000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>13.56</v>
       </c>
@@ -8529,8 +8663,11 @@
       <c r="AE42">
         <v>14.660238</v>
       </c>
-    </row>
-    <row r="43" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AG42" s="17">
+        <v>14.715389999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>13.56</v>
       </c>
@@ -8612,8 +8749,11 @@
       <c r="AE43">
         <v>50.016550000000002</v>
       </c>
-    </row>
-    <row r="44" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AG43" s="17">
+        <v>60.149340000000002</v>
+      </c>
+    </row>
+    <row r="44" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>13.56</v>
       </c>
@@ -8695,17 +8835,20 @@
       <c r="AE44">
         <v>17.565923999999999</v>
       </c>
-    </row>
-    <row r="45" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AG44" s="17">
+        <v>13.056656</v>
+      </c>
+    </row>
+    <row r="45" spans="1:33" x14ac:dyDescent="0.25">
       <c r="O45"/>
     </row>
-    <row r="46" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
       <c r="O46"/>
     </row>
-    <row r="47" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
       <c r="O47"/>
     </row>
-    <row r="48" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:33" x14ac:dyDescent="0.25">
       <c r="O48"/>
     </row>
     <row r="49" spans="15:15" x14ac:dyDescent="0.25">
@@ -8873,7 +9016,7 @@
       </c>
       <c r="I2">
         <f t="shared" ref="I2:I44" ca="1" si="0">RAND()</f>
-        <v>0.83873210254033503</v>
+        <v>0.99906670336062575</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -8903,7 +9046,7 @@
       </c>
       <c r="I3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.91203438733719944</v>
+        <v>0.33812211843564832</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -8933,7 +9076,7 @@
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.38369210886620109</v>
+        <v>0.24540033622153923</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -8963,7 +9106,7 @@
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.19578297585573201</v>
+        <v>0.38470854369673024</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -8993,7 +9136,7 @@
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.5965396396972017</v>
+        <v>0.26302177653546177</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -9023,7 +9166,7 @@
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.93308315688354349</v>
+        <v>0.46869881671549118</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -9053,7 +9196,7 @@
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="0"/>
-        <v>2.0065818675683467E-2</v>
+        <v>0.91188330323745159</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -9083,7 +9226,7 @@
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="0"/>
-        <v>0.27486153996181495</v>
+        <v>0.25920037254865314</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -9113,7 +9256,7 @@
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="0"/>
-        <v>0.15955509789232369</v>
+        <v>0.75371562707736983</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -9143,7 +9286,7 @@
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.69474005461427224</v>
+        <v>0.20123426977092851</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -9173,7 +9316,7 @@
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.81053106835802669</v>
+        <v>0.39038024868366306</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -9203,7 +9346,7 @@
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.63768693289181855</v>
+        <v>0.29100533228870773</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -9233,7 +9376,7 @@
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="0"/>
-        <v>0.59008504887741442</v>
+        <v>0.32016830505402294</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -9263,7 +9406,7 @@
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="0"/>
-        <v>0.88698177263046551</v>
+        <v>2.3195823508743385E-2</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -9293,7 +9436,7 @@
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.42487357812192927</v>
+        <v>0.91524066938423632</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -9323,7 +9466,7 @@
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="0"/>
-        <v>0.13899953937547438</v>
+        <v>0.66359105504288984</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -9353,7 +9496,7 @@
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="0"/>
-        <v>0.83572943787872855</v>
+        <v>0.38047189974228701</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -9383,7 +9526,7 @@
       </c>
       <c r="I19">
         <f t="shared" ca="1" si="0"/>
-        <v>0.82738188290525438</v>
+        <v>0.27273093660697179</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -9413,7 +9556,7 @@
       </c>
       <c r="I20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.35865687552824943</v>
+        <v>0.53349199751731646</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -9443,7 +9586,7 @@
       </c>
       <c r="I21">
         <f t="shared" ca="1" si="0"/>
-        <v>0.17969048305907087</v>
+        <v>0.91382697299611537</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -9473,7 +9616,7 @@
       </c>
       <c r="I22">
         <f t="shared" ca="1" si="0"/>
-        <v>0.49475801545512899</v>
+        <v>0.36426269610167561</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -9503,7 +9646,7 @@
       </c>
       <c r="I23">
         <f t="shared" ca="1" si="0"/>
-        <v>0.8819655892825129</v>
+        <v>0.76133585137071935</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -9533,7 +9676,7 @@
       </c>
       <c r="I24">
         <f t="shared" ca="1" si="0"/>
-        <v>0.80616255502656442</v>
+        <v>0.82958960420514827</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -9563,7 +9706,7 @@
       </c>
       <c r="I25">
         <f t="shared" ca="1" si="0"/>
-        <v>0.30538586130355794</v>
+        <v>0.54120159700681092</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -9593,7 +9736,7 @@
       </c>
       <c r="I26">
         <f t="shared" ca="1" si="0"/>
-        <v>0.89502435469379593</v>
+        <v>0.82481709301259498</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -9623,7 +9766,7 @@
       </c>
       <c r="I27">
         <f t="shared" ca="1" si="0"/>
-        <v>0.29084050152605789</v>
+        <v>0.56969346691535305</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -9653,7 +9796,7 @@
       </c>
       <c r="I28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.13044062353117192</v>
+        <v>0.95507363814815704</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -9683,7 +9826,7 @@
       </c>
       <c r="I29">
         <f t="shared" ca="1" si="0"/>
-        <v>0.16180439192492069</v>
+        <v>0.15510258628012918</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -9713,7 +9856,7 @@
       </c>
       <c r="I30">
         <f t="shared" ca="1" si="0"/>
-        <v>0.82265841391983296</v>
+        <v>3.4028512141351941E-2</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -9743,7 +9886,7 @@
       </c>
       <c r="I31">
         <f t="shared" ca="1" si="0"/>
-        <v>0.52948895600131152</v>
+        <v>0.97144830078265354</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -9773,7 +9916,7 @@
       </c>
       <c r="I32">
         <f t="shared" ca="1" si="0"/>
-        <v>0.71935395761582144</v>
+        <v>0.1399524819791601</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -9803,7 +9946,7 @@
       </c>
       <c r="I33">
         <f t="shared" ca="1" si="0"/>
-        <v>0.9526074395098364</v>
+        <v>7.8710771395573587E-2</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -9833,7 +9976,7 @@
       </c>
       <c r="I34">
         <f t="shared" ca="1" si="0"/>
-        <v>0.29982728105688317</v>
+        <v>0.27031493972240539</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -9863,7 +10006,7 @@
       </c>
       <c r="I35">
         <f t="shared" ca="1" si="0"/>
-        <v>0.3642736085109356</v>
+        <v>0.61047510035807195</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -9893,7 +10036,7 @@
       </c>
       <c r="I36">
         <f t="shared" ca="1" si="0"/>
-        <v>0.50735245136228491</v>
+        <v>0.36524404260652943</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -9923,7 +10066,7 @@
       </c>
       <c r="I37">
         <f t="shared" ca="1" si="0"/>
-        <v>0.81938936584099875</v>
+        <v>0.35995313462506606</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -9953,7 +10096,7 @@
       </c>
       <c r="I38">
         <f t="shared" ca="1" si="0"/>
-        <v>0.82895320848949638</v>
+        <v>0.59656143693393482</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -9983,7 +10126,7 @@
       </c>
       <c r="I39">
         <f t="shared" ca="1" si="0"/>
-        <v>0.64889787997240145</v>
+        <v>0.60868903144619402</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -10013,7 +10156,7 @@
       </c>
       <c r="I40">
         <f t="shared" ca="1" si="0"/>
-        <v>0.12730696012554232</v>
+        <v>4.1834023882683757E-2</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -10043,7 +10186,7 @@
       </c>
       <c r="I41">
         <f t="shared" ca="1" si="0"/>
-        <v>3.35372106985663E-2</v>
+        <v>0.91943358466218716</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -10073,7 +10216,7 @@
       </c>
       <c r="I42">
         <f t="shared" ca="1" si="0"/>
-        <v>0.44661231706008875</v>
+        <v>0.44837850462510542</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -10103,7 +10246,7 @@
       </c>
       <c r="I43">
         <f t="shared" ca="1" si="0"/>
-        <v>0.6121073651879011</v>
+        <v>5.668628750003335E-2</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -10133,7 +10276,7 @@
       </c>
       <c r="I44">
         <f t="shared" ca="1" si="0"/>
-        <v>0.20197328820573979</v>
+        <v>0.83595479011138341</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Best Prediction Model Committed
</commit_message>
<xml_diff>
--- a/results/4. NN_Regression/Data Set_NN.xlsx
+++ b/results/4. NN_Regression/Data Set_NN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GeonuKim\Desktop\ML project\Regression_Analysis_of_PECVD_SiNx\results\4. NN_Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C49AA6-3495-4D3B-A5D8-1F21B4740052}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E65320-4866-45C9-BC38-75FCD4847378}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="690" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Shuffled_Rand_removed" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
   <si>
     <t>RF Freq (MHz)</t>
   </si>
@@ -127,6 +127,15 @@
   <si>
     <t>Test_by_NN_Model_Ver1.1</t>
   </si>
+  <si>
+    <t>Test_by_NN_Model_Ver1.1_(10,000epochs, 2tanh+1linear)</t>
+  </si>
+  <si>
+    <t>Test_by_NN_Model_Ver1.1_(20,000epochs, 2tanh+1linear)</t>
+  </si>
+  <si>
+    <t>Test_by_NN_Model_Ver1.1_(50,000epochs, 2tanh+1linear)</t>
+  </si>
 </sst>
 </file>
 
@@ -169,7 +178,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -179,6 +188,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -228,7 +255,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -247,6 +274,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -582,133 +612,133 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="43"/>
                 <c:pt idx="0">
-                  <c:v>64.500429999999994</c:v>
+                  <c:v>317.58987000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>57.644629999999999</c:v>
+                  <c:v>53.364006000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-3.1444201000000001</c:v>
+                  <c:v>-2.632841</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24.484299</c:v>
+                  <c:v>25.884475999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>29.908297999999998</c:v>
+                  <c:v>27.519387999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17.387962000000002</c:v>
+                  <c:v>28.797909000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>112.05804999999999</c:v>
+                  <c:v>103.69773000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>24.664991000000001</c:v>
+                  <c:v>31.450078999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>123.306015</c:v>
+                  <c:v>106.20733</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>30.503983000000002</c:v>
+                  <c:v>32.968456000000003</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>16.606708999999999</c:v>
+                  <c:v>16.991379999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>104.72706599999999</c:v>
+                  <c:v>97.742189999999994</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>125.08148</c:v>
+                  <c:v>111.311424</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>98.083600000000004</c:v>
+                  <c:v>88.372649999999993</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>32.830275999999998</c:v>
+                  <c:v>27.477535</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>84.214516000000003</c:v>
+                  <c:v>82.262720000000002</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>118.32434000000001</c:v>
+                  <c:v>102.95579499999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>60.290030000000002</c:v>
+                  <c:v>76.161730000000006</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>32.119087</c:v>
+                  <c:v>34.129246000000002</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>41.246093999999999</c:v>
+                  <c:v>36.502422000000003</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>22.969854000000002</c:v>
+                  <c:v>23.085819999999998</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>57.373257000000002</c:v>
+                  <c:v>50.353928000000003</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>61.47636</c:v>
+                  <c:v>56.949249999999999</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>102.21980000000001</c:v>
+                  <c:v>91.419150000000002</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>8.9184479999999997</c:v>
+                  <c:v>7.9303913000000001</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>81.563469999999995</c:v>
+                  <c:v>74.987840000000006</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>77.887140000000002</c:v>
+                  <c:v>71.937979999999996</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>9.0806939999999994</c:v>
+                  <c:v>8.0779960000000006</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>143.82384999999999</c:v>
+                  <c:v>118.87919599999999</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>32.244624999999999</c:v>
+                  <c:v>34.271740000000001</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>139.24617000000001</c:v>
+                  <c:v>116.25306999999999</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>91.870159999999998</c:v>
+                  <c:v>89.251729999999995</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>44.392940000000003</c:v>
+                  <c:v>38.459060000000001</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>51.008395999999998</c:v>
+                  <c:v>54.072795999999997</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>43.351726999999997</c:v>
+                  <c:v>45.16892</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>10.144572</c:v>
+                  <c:v>9.404121</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>37.150016999999998</c:v>
+                  <c:v>32.180911999999999</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>-14.853265</c:v>
+                  <c:v>-13.376745</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>71.363715999999997</c:v>
+                  <c:v>72.663864000000004</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>50.658929999999998</c:v>
+                  <c:v>40.268172999999997</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>20.841923000000001</c:v>
+                  <c:v>17.911352000000001</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>64.139979999999994</c:v>
+                  <c:v>65.155760000000001</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>9.1597279999999994</c:v>
+                  <c:v>14.079703</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4580,13 +4610,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>394707</xdr:colOff>
+      <xdr:colOff>338678</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>119143</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>33927</xdr:colOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>583016</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>45428</xdr:rowOff>
     </xdr:to>
@@ -5037,10 +5067,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3186E75-438A-4A95-88D4-48D169AD77DA}">
-  <dimension ref="A1:AG89"/>
+  <dimension ref="A1:AK89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R19" sqref="R19"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R26" sqref="R26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5053,9 +5083,12 @@
     <col min="25" max="25" width="9.140625" style="12"/>
     <col min="28" max="28" width="9.140625" customWidth="1"/>
     <col min="33" max="33" width="9.140625" style="17"/>
+    <col min="35" max="35" width="9.140625" style="18"/>
+    <col min="36" max="36" width="9.140625" style="19"/>
+    <col min="37" max="37" width="9.140625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -5140,8 +5173,17 @@
       <c r="AG1" s="17" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI1" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ1" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="AK1" s="20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>13.56</v>
       </c>
@@ -5167,7 +5209,7 @@
         <v>317.68388106416199</v>
       </c>
       <c r="I2">
-        <v>64.500429999999994</v>
+        <v>317.58987000000002</v>
       </c>
       <c r="K2">
         <v>141.79940999999999</v>
@@ -5226,8 +5268,17 @@
       <c r="AG2" s="17">
         <v>68.751419999999996</v>
       </c>
-    </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI2" s="18">
+        <v>72.569659999999999</v>
+      </c>
+      <c r="AJ2" s="19">
+        <v>86.380250000000004</v>
+      </c>
+      <c r="AK2" s="20">
+        <v>317.58987000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>13.56</v>
       </c>
@@ -5253,7 +5304,7 @@
         <v>57.599999999999902</v>
       </c>
       <c r="I3">
-        <v>57.644629999999999</v>
+        <v>53.364006000000003</v>
       </c>
       <c r="K3">
         <v>86.042060000000006</v>
@@ -5312,8 +5363,17 @@
       <c r="AG3" s="17">
         <v>55.454532999999998</v>
       </c>
-    </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI3" s="18">
+        <v>53.228138000000001</v>
+      </c>
+      <c r="AJ3" s="19">
+        <v>59.307630000000003</v>
+      </c>
+      <c r="AK3" s="20">
+        <v>53.364006000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>13.56</v>
       </c>
@@ -5339,7 +5399,7 @@
         <v>-4.0938908485839596</v>
       </c>
       <c r="I4">
-        <v>-3.1444201000000001</v>
+        <v>-2.632841</v>
       </c>
       <c r="K4">
         <v>1.3984767</v>
@@ -5398,8 +5458,17 @@
       <c r="AG4" s="17">
         <v>-5.3729706000000004</v>
       </c>
-    </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI4" s="18">
+        <v>-9.3359749999999995</v>
+      </c>
+      <c r="AJ4" s="19">
+        <v>-4.1064705999999997</v>
+      </c>
+      <c r="AK4" s="20">
+        <v>-2.632841</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>13.56</v>
       </c>
@@ -5425,7 +5494,7 @@
         <v>16.626506024096301</v>
       </c>
       <c r="I5">
-        <v>24.484299</v>
+        <v>25.884475999999999</v>
       </c>
       <c r="K5">
         <v>43.953800000000001</v>
@@ -5484,8 +5553,17 @@
       <c r="AG5" s="17">
         <v>22.294035000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI5" s="18">
+        <v>20.647922999999999</v>
+      </c>
+      <c r="AJ5" s="19">
+        <v>20.886507000000002</v>
+      </c>
+      <c r="AK5" s="20">
+        <v>25.884475999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>13.56</v>
       </c>
@@ -5511,7 +5589,7 @@
         <v>31.7683881064162</v>
       </c>
       <c r="I6">
-        <v>29.908297999999998</v>
+        <v>27.519387999999999</v>
       </c>
       <c r="K6">
         <v>58.463752999999997</v>
@@ -5570,8 +5648,17 @@
       <c r="AG6" s="17">
         <v>33.027996000000002</v>
       </c>
-    </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI6" s="18">
+        <v>29.837557</v>
+      </c>
+      <c r="AJ6" s="19">
+        <v>39.355330000000002</v>
+      </c>
+      <c r="AK6" s="20">
+        <v>27.519387999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>13.56</v>
       </c>
@@ -5597,7 +5684,7 @@
         <v>25.094339622641499</v>
       </c>
       <c r="I7">
-        <v>17.387962000000002</v>
+        <v>28.797909000000001</v>
       </c>
       <c r="K7">
         <v>10.747189000000001</v>
@@ -5656,8 +5743,17 @@
       <c r="AG7" s="17">
         <v>34.922671999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI7" s="18">
+        <v>29.392005999999999</v>
+      </c>
+      <c r="AJ7" s="19">
+        <v>32.897669999999998</v>
+      </c>
+      <c r="AK7" s="20">
+        <v>28.797909000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>13.56</v>
       </c>
@@ -5683,7 +5779,7 @@
         <v>148.14814814814801</v>
       </c>
       <c r="I8">
-        <v>112.05804999999999</v>
+        <v>103.69773000000001</v>
       </c>
       <c r="K8">
         <v>74.803825000000003</v>
@@ -5742,8 +5838,17 @@
       <c r="AG8" s="17">
         <v>126.76423</v>
       </c>
-    </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI8" s="18">
+        <v>146.78110000000001</v>
+      </c>
+      <c r="AJ8" s="19">
+        <v>142.56688</v>
+      </c>
+      <c r="AK8" s="20">
+        <v>103.69773000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>13.56</v>
       </c>
@@ -5769,7 +5874,7 @@
         <v>35.951972555746103</v>
       </c>
       <c r="I9">
-        <v>24.664991000000001</v>
+        <v>31.450078999999999</v>
       </c>
       <c r="K9">
         <v>33.165764000000003</v>
@@ -5828,8 +5933,17 @@
       <c r="AG9" s="17">
         <v>30.668865</v>
       </c>
-    </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI9" s="18">
+        <v>32.982979999999998</v>
+      </c>
+      <c r="AJ9" s="19">
+        <v>34.588253000000002</v>
+      </c>
+      <c r="AK9" s="20">
+        <v>31.450078999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>13.56</v>
       </c>
@@ -5855,7 +5969,7 @@
         <v>94.340740740740699</v>
       </c>
       <c r="I10">
-        <v>123.306015</v>
+        <v>106.20733</v>
       </c>
       <c r="K10">
         <v>125.39037999999999</v>
@@ -5914,8 +6028,17 @@
       <c r="AG10" s="17">
         <v>112.17992</v>
       </c>
-    </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI10" s="18">
+        <v>102.76136</v>
+      </c>
+      <c r="AJ10" s="19">
+        <v>93.695305000000005</v>
+      </c>
+      <c r="AK10" s="20">
+        <v>106.20733</v>
+      </c>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>13.56</v>
       </c>
@@ -5941,7 +6064,7 @@
         <v>27.970370370370301</v>
       </c>
       <c r="I11">
-        <v>30.503983000000002</v>
+        <v>32.968456000000003</v>
       </c>
       <c r="K11">
         <v>31.763824</v>
@@ -6000,8 +6123,17 @@
       <c r="AG11" s="17">
         <v>27.497883000000002</v>
       </c>
-    </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI11" s="18">
+        <v>24.168717999999998</v>
+      </c>
+      <c r="AJ11" s="19">
+        <v>21.093976999999999</v>
+      </c>
+      <c r="AK11" s="20">
+        <v>32.968456000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>13.56</v>
       </c>
@@ -6027,7 +6159,7 @@
         <v>3.25301204819276</v>
       </c>
       <c r="I12">
-        <v>16.606708999999999</v>
+        <v>16.991379999999999</v>
       </c>
       <c r="K12">
         <v>31.411884000000001</v>
@@ -6086,8 +6218,17 @@
       <c r="AG12" s="17">
         <v>13.376815000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI12" s="18">
+        <v>7.2026972999999996</v>
+      </c>
+      <c r="AJ12" s="19">
+        <v>6.1510496000000003</v>
+      </c>
+      <c r="AK12" s="20">
+        <v>16.991379999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>13.56</v>
       </c>
@@ -6113,7 +6254,7 @@
         <v>90.311111111111103</v>
       </c>
       <c r="I13">
-        <v>104.72706599999999</v>
+        <v>97.742189999999994</v>
       </c>
       <c r="K13">
         <v>85.033905000000004</v>
@@ -6172,8 +6313,17 @@
       <c r="AG13" s="17">
         <v>100.48035</v>
       </c>
-    </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI13" s="18">
+        <v>95.214219999999997</v>
+      </c>
+      <c r="AJ13" s="19">
+        <v>96.177620000000005</v>
+      </c>
+      <c r="AK13" s="20">
+        <v>97.742189999999994</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>13.56</v>
       </c>
@@ -6199,7 +6349,7 @@
         <v>118.992592592592</v>
       </c>
       <c r="I14">
-        <v>125.08148</v>
+        <v>111.311424</v>
       </c>
       <c r="K14">
         <v>95.775925000000001</v>
@@ -6258,8 +6408,17 @@
       <c r="AG14" s="17">
         <v>122.66893</v>
       </c>
-    </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI14" s="18">
+        <v>119.29237000000001</v>
+      </c>
+      <c r="AJ14" s="19">
+        <v>122.24121</v>
+      </c>
+      <c r="AK14" s="20">
+        <v>111.311424</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>13.56</v>
       </c>
@@ -6285,7 +6444,7 @@
         <v>97.896296296296299</v>
       </c>
       <c r="I15">
-        <v>98.083600000000004</v>
+        <v>88.372649999999993</v>
       </c>
       <c r="K15">
         <v>107.38366000000001</v>
@@ -6344,8 +6503,17 @@
       <c r="AG15" s="17">
         <v>88.287270000000007</v>
       </c>
-    </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI15" s="18">
+        <v>84.506439999999998</v>
+      </c>
+      <c r="AJ15" s="19">
+        <v>83.373726000000005</v>
+      </c>
+      <c r="AK15" s="20">
+        <v>88.372649999999993</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>13.56</v>
       </c>
@@ -6371,7 +6539,7 @@
         <v>22.7236147432425</v>
       </c>
       <c r="I16">
-        <v>32.830275999999998</v>
+        <v>27.477535</v>
       </c>
       <c r="K16">
         <v>54.411000000000001</v>
@@ -6430,8 +6598,17 @@
       <c r="AG16" s="17">
         <v>24.917252999999999</v>
       </c>
-    </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI16" s="18">
+        <v>29.891949</v>
+      </c>
+      <c r="AJ16" s="19">
+        <v>31.420666000000001</v>
+      </c>
+      <c r="AK16" s="20">
+        <v>27.477535</v>
+      </c>
+    </row>
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>13.56</v>
       </c>
@@ -6457,7 +6634,7 @@
         <v>79.170370370370307</v>
       </c>
       <c r="I17">
-        <v>84.214516000000003</v>
+        <v>82.262720000000002</v>
       </c>
       <c r="K17">
         <v>74.208439999999996</v>
@@ -6516,8 +6693,17 @@
       <c r="AG17" s="17">
         <v>79.326099999999997</v>
       </c>
-    </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI17" s="18">
+        <v>73.871579999999994</v>
+      </c>
+      <c r="AJ17" s="19">
+        <v>75.069209999999998</v>
+      </c>
+      <c r="AK17" s="20">
+        <v>82.262720000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>13.56</v>
       </c>
@@ -6543,7 +6729,7 @@
         <v>93.629629629629605</v>
       </c>
       <c r="I18">
-        <v>118.32434000000001</v>
+        <v>102.95579499999999</v>
       </c>
       <c r="K18">
         <v>118.065674</v>
@@ -6602,8 +6788,17 @@
       <c r="AG18" s="17">
         <v>106.89429</v>
       </c>
-    </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI18" s="18">
+        <v>102.22841</v>
+      </c>
+      <c r="AJ18" s="19">
+        <v>98.292529999999999</v>
+      </c>
+      <c r="AK18" s="20">
+        <v>102.95579499999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>13.56</v>
       </c>
@@ -6629,7 +6824,7 @@
         <v>76.134585289514902</v>
       </c>
       <c r="I19">
-        <v>60.290030000000002</v>
+        <v>76.161730000000006</v>
       </c>
       <c r="K19">
         <v>131.65619000000001</v>
@@ -6688,8 +6883,17 @@
       <c r="AG19" s="17">
         <v>64.694360000000003</v>
       </c>
-    </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI19" s="18">
+        <v>67.454155</v>
+      </c>
+      <c r="AJ19" s="19">
+        <v>80.75985</v>
+      </c>
+      <c r="AK19" s="20">
+        <v>76.161730000000006</v>
+      </c>
+    </row>
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>13.56</v>
       </c>
@@ -6715,7 +6919,7 @@
         <v>40.068610634648302</v>
       </c>
       <c r="I20">
-        <v>32.119087</v>
+        <v>34.129246000000002</v>
       </c>
       <c r="K20">
         <v>56.129795000000001</v>
@@ -6774,8 +6978,17 @@
       <c r="AG20" s="17">
         <v>30.91028</v>
       </c>
-    </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI20" s="18">
+        <v>36.693989999999999</v>
+      </c>
+      <c r="AJ20" s="19">
+        <v>37.738030000000002</v>
+      </c>
+      <c r="AK20" s="20">
+        <v>34.129246000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>13.56</v>
       </c>
@@ -6801,7 +7014,7 @@
         <v>60.681481481481399</v>
       </c>
       <c r="I21">
-        <v>41.246093999999999</v>
+        <v>36.502422000000003</v>
       </c>
       <c r="K21">
         <v>82.083404999999999</v>
@@ -6860,8 +7073,17 @@
       <c r="AG21" s="17">
         <v>45.266629999999999</v>
       </c>
-    </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI21" s="18">
+        <v>46.553604</v>
+      </c>
+      <c r="AJ21" s="19">
+        <v>55.315514</v>
+      </c>
+      <c r="AK21" s="20">
+        <v>36.502422000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>13.56</v>
       </c>
@@ -6887,7 +7109,7 @@
         <v>36.977777777777703</v>
       </c>
       <c r="I22">
-        <v>22.969854000000002</v>
+        <v>23.085819999999998</v>
       </c>
       <c r="K22">
         <v>41.886684000000002</v>
@@ -6946,8 +7168,17 @@
       <c r="AG22" s="17">
         <v>25.980103</v>
       </c>
-    </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI22" s="18">
+        <v>21.337164000000001</v>
+      </c>
+      <c r="AJ22" s="19">
+        <v>30.276651000000001</v>
+      </c>
+      <c r="AK22" s="20">
+        <v>23.085819999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>13.56</v>
       </c>
@@ -6973,7 +7204,7 @@
         <v>62.9890453834116</v>
       </c>
       <c r="I23">
-        <v>57.373257000000002</v>
+        <v>50.353928000000003</v>
       </c>
       <c r="K23">
         <v>124.62942</v>
@@ -7032,8 +7263,17 @@
       <c r="AG23" s="17">
         <v>61.799045999999997</v>
       </c>
-    </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI23" s="18">
+        <v>63.886699999999998</v>
+      </c>
+      <c r="AJ23" s="19">
+        <v>76.830123999999998</v>
+      </c>
+      <c r="AK23" s="20">
+        <v>50.353928000000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>13.56</v>
       </c>
@@ -7059,7 +7299,7 @@
         <v>68.740740740740705</v>
       </c>
       <c r="I24">
-        <v>61.47636</v>
+        <v>56.949249999999999</v>
       </c>
       <c r="K24">
         <v>92.759895</v>
@@ -7118,8 +7358,17 @@
       <c r="AG24" s="17">
         <v>59.996014000000002</v>
       </c>
-    </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI24" s="18">
+        <v>59.678150000000002</v>
+      </c>
+      <c r="AJ24" s="19">
+        <v>63.972866000000003</v>
+      </c>
+      <c r="AK24" s="20">
+        <v>56.949249999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>13.56</v>
       </c>
@@ -7145,7 +7394,7 @@
         <v>87.229629629629599</v>
       </c>
       <c r="I25">
-        <v>102.21980000000001</v>
+        <v>91.419150000000002</v>
       </c>
       <c r="K25">
         <v>114.26217</v>
@@ -7204,8 +7453,17 @@
       <c r="AG25" s="17">
         <v>92.902169999999998</v>
       </c>
-    </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI25" s="18">
+        <v>87.268569999999997</v>
+      </c>
+      <c r="AJ25" s="19">
+        <v>82.711939999999998</v>
+      </c>
+      <c r="AK25" s="20">
+        <v>91.419150000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>13.56</v>
       </c>
@@ -7231,7 +7489,7 @@
         <v>-8.3855421686747</v>
       </c>
       <c r="I26">
-        <v>8.9184479999999997</v>
+        <v>7.9303913000000001</v>
       </c>
       <c r="K26">
         <v>19.171399999999998</v>
@@ -7290,8 +7548,17 @@
       <c r="AG26" s="17">
         <v>4.6627280000000004</v>
       </c>
-    </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI26" s="18">
+        <v>1.8797166000000001</v>
+      </c>
+      <c r="AJ26" s="19">
+        <v>4.6791970000000003</v>
+      </c>
+      <c r="AK26" s="20">
+        <v>7.9303913000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>13.56</v>
       </c>
@@ -7317,7 +7584,7 @@
         <v>77.511111111111106</v>
       </c>
       <c r="I27">
-        <v>81.563469999999995</v>
+        <v>74.987840000000006</v>
       </c>
       <c r="K27">
         <v>103.36082500000001</v>
@@ -7376,8 +7643,17 @@
       <c r="AG27" s="17">
         <v>75.546239999999997</v>
       </c>
-    </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI27" s="18">
+        <v>73.007339999999999</v>
+      </c>
+      <c r="AJ27" s="19">
+        <v>72.916600000000003</v>
+      </c>
+      <c r="AK27" s="20">
+        <v>74.987840000000006</v>
+      </c>
+    </row>
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>13.56</v>
       </c>
@@ -7403,7 +7679,7 @@
         <v>51.911111111111097</v>
       </c>
       <c r="I28">
-        <v>77.887140000000002</v>
+        <v>71.937979999999996</v>
       </c>
       <c r="K28">
         <v>96.724999999999994</v>
@@ -7462,8 +7738,17 @@
       <c r="AG28" s="17">
         <v>71.204864999999998</v>
       </c>
-    </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI28" s="18">
+        <v>68.353499999999997</v>
+      </c>
+      <c r="AJ28" s="19">
+        <v>70.622420000000005</v>
+      </c>
+      <c r="AK28" s="20">
+        <v>71.937979999999996</v>
+      </c>
+    </row>
+    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>13.56</v>
       </c>
@@ -7489,7 +7774,7 @@
         <v>8.8974836132918291</v>
       </c>
       <c r="I29">
-        <v>9.0806939999999994</v>
+        <v>8.0779960000000006</v>
       </c>
       <c r="K29">
         <v>19.413471000000001</v>
@@ -7548,8 +7833,17 @@
       <c r="AG29" s="17">
         <v>4.8061290000000003</v>
       </c>
-    </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI29" s="18">
+        <v>2.0180660000000001</v>
+      </c>
+      <c r="AJ29" s="19">
+        <v>4.7607865</v>
+      </c>
+      <c r="AK29" s="20">
+        <v>8.0779960000000006</v>
+      </c>
+    </row>
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>13.56</v>
       </c>
@@ -7575,7 +7869,7 @@
         <v>99.5555555555555</v>
       </c>
       <c r="I30">
-        <v>143.82384999999999</v>
+        <v>118.87919599999999</v>
       </c>
       <c r="K30">
         <v>136.21861000000001</v>
@@ -7634,8 +7928,17 @@
       <c r="AG30" s="17">
         <v>132.30789999999999</v>
       </c>
-    </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI30" s="18">
+        <v>119.20034</v>
+      </c>
+      <c r="AJ30" s="19">
+        <v>105.83195000000001</v>
+      </c>
+      <c r="AK30" s="20">
+        <v>118.87919599999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>13.56</v>
       </c>
@@ -7661,7 +7964,7 @@
         <v>26.024096385542101</v>
       </c>
       <c r="I31">
-        <v>32.244624999999999</v>
+        <v>34.271740000000001</v>
       </c>
       <c r="K31">
         <v>56.309024999999998</v>
@@ -7720,8 +8023,17 @@
       <c r="AG31" s="17">
         <v>31.062002</v>
       </c>
-    </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI31" s="18">
+        <v>36.992263999999999</v>
+      </c>
+      <c r="AJ31" s="19">
+        <v>38.042941999999996</v>
+      </c>
+      <c r="AK31" s="20">
+        <v>34.271740000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>13.56</v>
       </c>
@@ -7747,7 +8059,7 @@
         <v>125.86666666666601</v>
       </c>
       <c r="I32">
-        <v>139.24617000000001</v>
+        <v>116.25306999999999</v>
       </c>
       <c r="K32">
         <v>129.10712000000001</v>
@@ -7806,8 +8118,17 @@
       <c r="AG32" s="17">
         <v>127.54550999999999</v>
       </c>
-    </row>
-    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI32" s="18">
+        <v>122.77218999999999</v>
+      </c>
+      <c r="AJ32" s="19">
+        <v>116.94083000000001</v>
+      </c>
+      <c r="AK32" s="20">
+        <v>116.25306999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>13.56</v>
       </c>
@@ -7833,7 +8154,7 @@
         <v>92.4444444444444</v>
       </c>
       <c r="I33">
-        <v>91.870159999999998</v>
+        <v>89.251729999999995</v>
       </c>
       <c r="K33">
         <v>64.149720000000002</v>
@@ -7892,8 +8213,17 @@
       <c r="AG33" s="17">
         <v>101.22172500000001</v>
       </c>
-    </row>
-    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI33" s="18">
+        <v>110.51595</v>
+      </c>
+      <c r="AJ33" s="19">
+        <v>101.76088</v>
+      </c>
+      <c r="AK33" s="20">
+        <v>89.251729999999995</v>
+      </c>
+    </row>
+    <row r="34" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>13.56</v>
       </c>
@@ -7919,7 +8249,7 @@
         <v>44.030874785591699</v>
       </c>
       <c r="I34">
-        <v>44.392940000000003</v>
+        <v>38.459060000000001</v>
       </c>
       <c r="K34">
         <v>93.942245</v>
@@ -7978,8 +8308,17 @@
       <c r="AG34" s="17">
         <v>43.221989999999998</v>
       </c>
-    </row>
-    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI34" s="18">
+        <v>42.847496</v>
+      </c>
+      <c r="AJ34" s="19">
+        <v>43.758110000000002</v>
+      </c>
+      <c r="AK34" s="20">
+        <v>38.459060000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>13.56</v>
       </c>
@@ -8005,7 +8344,7 @@
         <v>48.118518518518499</v>
       </c>
       <c r="I35">
-        <v>51.008395999999998</v>
+        <v>54.072795999999997</v>
       </c>
       <c r="K35">
         <v>42.584980000000002</v>
@@ -8064,8 +8403,17 @@
       <c r="AG35" s="17">
         <v>50.949820000000003</v>
       </c>
-    </row>
-    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI35" s="18">
+        <v>49.348945999999998</v>
+      </c>
+      <c r="AJ35" s="19">
+        <v>42.581783000000001</v>
+      </c>
+      <c r="AK35" s="20">
+        <v>54.072795999999997</v>
+      </c>
+    </row>
+    <row r="36" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>13.56</v>
       </c>
@@ -8091,7 +8439,7 @@
         <v>35.318518518518403</v>
       </c>
       <c r="I36">
-        <v>43.351726999999997</v>
+        <v>45.16892</v>
       </c>
       <c r="K36">
         <v>52.643191999999999</v>
@@ -8150,8 +8498,17 @@
       <c r="AG36" s="17">
         <v>42.059852999999997</v>
       </c>
-    </row>
-    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI36" s="18">
+        <v>37.500453999999998</v>
+      </c>
+      <c r="AJ36" s="19">
+        <v>43.103713999999997</v>
+      </c>
+      <c r="AK36" s="20">
+        <v>45.16892</v>
+      </c>
+    </row>
+    <row r="37" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>13.56</v>
       </c>
@@ -8177,7 +8534,7 @@
         <v>4.9777777777777601</v>
       </c>
       <c r="I37">
-        <v>10.144572</v>
+        <v>9.404121</v>
       </c>
       <c r="K37">
         <v>21.019169999999999</v>
@@ -8236,8 +8593,17 @@
       <c r="AG37" s="17">
         <v>6.0401315999999996</v>
       </c>
-    </row>
-    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI37" s="18">
+        <v>1.9965402999999999</v>
+      </c>
+      <c r="AJ37" s="19">
+        <v>3.270683</v>
+      </c>
+      <c r="AK37" s="20">
+        <v>9.404121</v>
+      </c>
+    </row>
+    <row r="38" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>13.56</v>
       </c>
@@ -8263,7 +8629,7 @@
         <v>26.311111111111099</v>
       </c>
       <c r="I38">
-        <v>37.150016999999998</v>
+        <v>32.180911999999999</v>
       </c>
       <c r="K38">
         <v>75.226060000000004</v>
@@ -8322,8 +8688,17 @@
       <c r="AG38" s="17">
         <v>40.512529999999998</v>
       </c>
-    </row>
-    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI38" s="18">
+        <v>38.628456</v>
+      </c>
+      <c r="AJ38" s="19">
+        <v>48.848790000000001</v>
+      </c>
+      <c r="AK38" s="20">
+        <v>32.180911999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>13.56</v>
       </c>
@@ -8349,7 +8724,7 @@
         <v>-17.334986043112099</v>
       </c>
       <c r="I39">
-        <v>-14.853265</v>
+        <v>-13.376745</v>
       </c>
       <c r="K39">
         <v>-15.855751</v>
@@ -8408,8 +8783,17 @@
       <c r="AG39" s="17">
         <v>-14.991389</v>
       </c>
-    </row>
-    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI39" s="18">
+        <v>-17.25102</v>
+      </c>
+      <c r="AJ39" s="19">
+        <v>-6.8277099999999997</v>
+      </c>
+      <c r="AK39" s="20">
+        <v>-13.376745</v>
+      </c>
+    </row>
+    <row r="40" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>13.56</v>
       </c>
@@ -8435,7 +8819,7 @@
         <v>75.614814814814807</v>
       </c>
       <c r="I40">
-        <v>71.363715999999997</v>
+        <v>72.663864000000004</v>
       </c>
       <c r="K40">
         <v>53.327464999999997</v>
@@ -8494,8 +8878,17 @@
       <c r="AG40" s="17">
         <v>75.581695999999994</v>
       </c>
-    </row>
-    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI40" s="18">
+        <v>77.8215</v>
+      </c>
+      <c r="AJ40" s="19">
+        <v>68.778403999999995</v>
+      </c>
+      <c r="AK40" s="20">
+        <v>72.663864000000004</v>
+      </c>
+    </row>
+    <row r="41" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>13.56</v>
       </c>
@@ -8521,7 +8914,7 @@
         <v>44.913928012519499</v>
       </c>
       <c r="I41">
-        <v>50.658929999999998</v>
+        <v>40.268172999999997</v>
       </c>
       <c r="K41">
         <v>108.45395000000001</v>
@@ -8580,8 +8973,17 @@
       <c r="AG41" s="17">
         <v>54.924610000000001</v>
       </c>
-    </row>
-    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI41" s="18">
+        <v>55.613852999999999</v>
+      </c>
+      <c r="AJ41" s="19">
+        <v>67.695369999999997</v>
+      </c>
+      <c r="AK41" s="20">
+        <v>40.268172999999997</v>
+      </c>
+    </row>
+    <row r="42" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>13.56</v>
       </c>
@@ -8607,7 +9009,7 @@
         <v>14.870500296762</v>
       </c>
       <c r="I42">
-        <v>20.841923000000001</v>
+        <v>17.911352000000001</v>
       </c>
       <c r="K42">
         <v>36.744889999999998</v>
@@ -8666,8 +9068,17 @@
       <c r="AG42" s="17">
         <v>14.715389999999999</v>
       </c>
-    </row>
-    <row r="43" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI42" s="18">
+        <v>15.108936999999999</v>
+      </c>
+      <c r="AJ42" s="19">
+        <v>16.926582</v>
+      </c>
+      <c r="AK42" s="20">
+        <v>17.911352000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>13.56</v>
       </c>
@@ -8693,7 +9104,7 @@
         <v>57.362962962962897</v>
       </c>
       <c r="I43">
-        <v>64.139979999999994</v>
+        <v>65.155760000000001</v>
       </c>
       <c r="K43">
         <v>63.614139999999999</v>
@@ -8752,8 +9163,17 @@
       <c r="AG43" s="17">
         <v>60.149340000000002</v>
       </c>
-    </row>
-    <row r="44" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI43" s="18">
+        <v>55.178379999999997</v>
+      </c>
+      <c r="AJ43" s="19">
+        <v>58.049995000000003</v>
+      </c>
+      <c r="AK43" s="20">
+        <v>65.155760000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>13.56</v>
       </c>
@@ -8779,7 +9199,7 @@
         <v>26.8388106416275</v>
       </c>
       <c r="I44">
-        <v>9.1597279999999994</v>
+        <v>14.079703</v>
       </c>
       <c r="K44">
         <v>8.4785179999999993</v>
@@ -8838,17 +9258,26 @@
       <c r="AG44" s="17">
         <v>13.056656</v>
       </c>
-    </row>
-    <row r="45" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI44" s="18">
+        <v>4.8166924</v>
+      </c>
+      <c r="AJ44" s="19">
+        <v>13.688307999999999</v>
+      </c>
+      <c r="AK44" s="20">
+        <v>14.079703</v>
+      </c>
+    </row>
+    <row r="45" spans="1:37" x14ac:dyDescent="0.25">
       <c r="O45"/>
     </row>
-    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:37" x14ac:dyDescent="0.25">
       <c r="O46"/>
     </row>
-    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:37" x14ac:dyDescent="0.25">
       <c r="O47"/>
     </row>
-    <row r="48" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:37" x14ac:dyDescent="0.25">
       <c r="O48"/>
     </row>
     <row r="49" spans="15:15" x14ac:dyDescent="0.25">
@@ -9016,7 +9445,7 @@
       </c>
       <c r="I2">
         <f t="shared" ref="I2:I44" ca="1" si="0">RAND()</f>
-        <v>0.99906670336062575</v>
+        <v>0.12097180494310222</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -9046,7 +9475,7 @@
       </c>
       <c r="I3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.33812211843564832</v>
+        <v>0.77114491735384116</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -9076,7 +9505,7 @@
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.24540033622153923</v>
+        <v>0.32249748984507043</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -9106,7 +9535,7 @@
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.38470854369673024</v>
+        <v>0.99010516574972351</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -9136,7 +9565,7 @@
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.26302177653546177</v>
+        <v>0.10089095667900461</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -9166,7 +9595,7 @@
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.46869881671549118</v>
+        <v>0.30782715019464113</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -9196,7 +9625,7 @@
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.91188330323745159</v>
+        <v>0.75876117622900696</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -9226,7 +9655,7 @@
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="0"/>
-        <v>0.25920037254865314</v>
+        <v>0.2122815853832567</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -9256,7 +9685,7 @@
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="0"/>
-        <v>0.75371562707736983</v>
+        <v>0.65864792920940995</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -9286,7 +9715,7 @@
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.20123426977092851</v>
+        <v>0.24306806208058951</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -9316,7 +9745,7 @@
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.39038024868366306</v>
+        <v>0.19486611385131924</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -9346,7 +9775,7 @@
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.29100533228870773</v>
+        <v>0.1320700615059448</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -9376,7 +9805,7 @@
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="0"/>
-        <v>0.32016830505402294</v>
+        <v>0.48569519579452447</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -9406,7 +9835,7 @@
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="0"/>
-        <v>2.3195823508743385E-2</v>
+        <v>0.78351954870684692</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -9436,7 +9865,7 @@
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.91524066938423632</v>
+        <v>0.72514111352722743</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -9466,7 +9895,7 @@
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="0"/>
-        <v>0.66359105504288984</v>
+        <v>0.62555874262642819</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -9496,7 +9925,7 @@
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="0"/>
-        <v>0.38047189974228701</v>
+        <v>0.27460315428718218</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -9526,7 +9955,7 @@
       </c>
       <c r="I19">
         <f t="shared" ca="1" si="0"/>
-        <v>0.27273093660697179</v>
+        <v>0.78397038747913295</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -9556,7 +9985,7 @@
       </c>
       <c r="I20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.53349199751731646</v>
+        <v>0.87786779793491143</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -9586,7 +10015,7 @@
       </c>
       <c r="I21">
         <f t="shared" ca="1" si="0"/>
-        <v>0.91382697299611537</v>
+        <v>0.12942055563286325</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -9616,7 +10045,7 @@
       </c>
       <c r="I22">
         <f t="shared" ca="1" si="0"/>
-        <v>0.36426269610167561</v>
+        <v>0.14714737635307662</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -9646,7 +10075,7 @@
       </c>
       <c r="I23">
         <f t="shared" ca="1" si="0"/>
-        <v>0.76133585137071935</v>
+        <v>0.3834220658189158</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -9676,7 +10105,7 @@
       </c>
       <c r="I24">
         <f t="shared" ca="1" si="0"/>
-        <v>0.82958960420514827</v>
+        <v>1.7957413441879067E-2</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -9706,7 +10135,7 @@
       </c>
       <c r="I25">
         <f t="shared" ca="1" si="0"/>
-        <v>0.54120159700681092</v>
+        <v>0.13537784623679472</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -9736,7 +10165,7 @@
       </c>
       <c r="I26">
         <f t="shared" ca="1" si="0"/>
-        <v>0.82481709301259498</v>
+        <v>0.55103554905127294</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -9766,7 +10195,7 @@
       </c>
       <c r="I27">
         <f t="shared" ca="1" si="0"/>
-        <v>0.56969346691535305</v>
+        <v>0.10009170469503959</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -9796,7 +10225,7 @@
       </c>
       <c r="I28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.95507363814815704</v>
+        <v>0.50824080956876483</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -9826,7 +10255,7 @@
       </c>
       <c r="I29">
         <f t="shared" ca="1" si="0"/>
-        <v>0.15510258628012918</v>
+        <v>0.49161244389290626</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -9856,7 +10285,7 @@
       </c>
       <c r="I30">
         <f t="shared" ca="1" si="0"/>
-        <v>3.4028512141351941E-2</v>
+        <v>0.69980130286650555</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -9886,7 +10315,7 @@
       </c>
       <c r="I31">
         <f t="shared" ca="1" si="0"/>
-        <v>0.97144830078265354</v>
+        <v>0.32302189416068505</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -9916,7 +10345,7 @@
       </c>
       <c r="I32">
         <f t="shared" ca="1" si="0"/>
-        <v>0.1399524819791601</v>
+        <v>0.42598865075625725</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -9946,7 +10375,7 @@
       </c>
       <c r="I33">
         <f t="shared" ca="1" si="0"/>
-        <v>7.8710771395573587E-2</v>
+        <v>0.53996429328644169</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -9976,7 +10405,7 @@
       </c>
       <c r="I34">
         <f t="shared" ca="1" si="0"/>
-        <v>0.27031493972240539</v>
+        <v>0.17784839413006825</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -10006,7 +10435,7 @@
       </c>
       <c r="I35">
         <f t="shared" ca="1" si="0"/>
-        <v>0.61047510035807195</v>
+        <v>0.86279098582149949</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -10036,7 +10465,7 @@
       </c>
       <c r="I36">
         <f t="shared" ca="1" si="0"/>
-        <v>0.36524404260652943</v>
+        <v>0.20810780998836076</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -10066,7 +10495,7 @@
       </c>
       <c r="I37">
         <f t="shared" ca="1" si="0"/>
-        <v>0.35995313462506606</v>
+        <v>0.49999991759765683</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -10096,7 +10525,7 @@
       </c>
       <c r="I38">
         <f t="shared" ca="1" si="0"/>
-        <v>0.59656143693393482</v>
+        <v>0.29106792327527242</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -10126,7 +10555,7 @@
       </c>
       <c r="I39">
         <f t="shared" ca="1" si="0"/>
-        <v>0.60868903144619402</v>
+        <v>0.60783814024825655</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -10156,7 +10585,7 @@
       </c>
       <c r="I40">
         <f t="shared" ca="1" si="0"/>
-        <v>4.1834023882683757E-2</v>
+        <v>0.57958010447643871</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -10186,7 +10615,7 @@
       </c>
       <c r="I41">
         <f t="shared" ca="1" si="0"/>
-        <v>0.91943358466218716</v>
+        <v>0.59264675614103746</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -10216,7 +10645,7 @@
       </c>
       <c r="I42">
         <f t="shared" ca="1" si="0"/>
-        <v>0.44837850462510542</v>
+        <v>0.84898190665720985</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -10246,7 +10675,7 @@
       </c>
       <c r="I43">
         <f t="shared" ca="1" si="0"/>
-        <v>5.668628750003335E-2</v>
+        <v>0.63168494350444193</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -10276,7 +10705,7 @@
       </c>
       <c r="I44">
         <f t="shared" ca="1" si="0"/>
-        <v>0.83595479011138341</v>
+        <v>0.49563054682976104</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -10294,7 +10723,7 @@
   <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31:H36"/>
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>